<commit_message>
Update notebook and experiment csv
</commit_message>
<xml_diff>
--- a/experiment_tracker.xlsx
+++ b/experiment_tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Data Vault\GitHub\Data-Centric-AI-Competition-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Data Vault\GitHub\Data-Centric-AI-Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -41,51 +41,10 @@
     <t>Bundle failed</t>
   </si>
   <si>
-    <t xml:space="preserve">• Simple initial augmentations with random affine and color jitter
-• Random affine and color jitter for all labels (I to X)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Start data shuffle of train and val raw folders, and then finally do a  random split 70/30 to train/val after augmentation complete
-• Use imgaug library instead of Torchvision
-• Implement imgaug's proposed simple augmentation sequence (https://imgaug.readthedocs.io/en/latest/source/examples_basics.html#a-simple-and-common-augmentation-sequence)
-• Perform random horizontal flip for labels i, ii, iii, v, x
-</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">• No pre-processing (Baseline)
-</t>
-  </si>
-  <si>
     <t>Improvement from Last</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Repeat steps (e.g. data shuffle and baseline imgaug basic augmentation, train test split 70/30) from Experiment 2
-• Introduce random vertical flips for i,ii, iii, ix, x
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Remove random order of augmentation (i.e. keep augmentation steps sequential in pre-specified order)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Perform extensive manual review of data (i.e. review past deleted images and add back if looks valid, while also reviewing existing ones to check that they are correctly labeled
-• Add sample label book data into training set
-• Adjust train/val split from 70/30 to 80/20
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Reinstate random order of augmentation
-• Adjust train/val split from 80/20 to 90/10
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Re-use steps from Experiment 4
-• Include CV2 morphological operations e.g. random erosion and dilation
-</t>
   </si>
   <si>
     <t xml:space="preserve">• Re-use steps from Experiment 6
@@ -102,6 +61,55 @@
 • Increase image size from 400x400 to 500x500
 • Run more in depth augmentation (e.g. include random perspective transform, reduce additivegaussian noise, increase rotation angle, increase multiply range)
 </t>
+  </si>
+  <si>
+    <t>Train/Test Split</t>
+  </si>
+  <si>
+    <t>70/30</t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>90/10</t>
+  </si>
+  <si>
+    <t>97.5/2.5</t>
+  </si>
+  <si>
+    <t>• Start data shuffle of train and val raw folders, and then finally do a  random split 70/30 to train/val after augmentation complete
+• Switch to imgaug library instead of Torchvision
+• Implement imgaug's proposed simple augmentation sequence (https://imgaug.readthedocs.io/en/latest/source/examples_basics.html#a-simple-and-common-augmentation-sequence)
+• Perform random horizontal flip for labels i, ii, iii, v, x</t>
+  </si>
+  <si>
+    <t>• Simple initial augmentations with random affine and color jitter
+• Random affine and color jitter for all labels (I to X)
+• Data cleaning initiated</t>
+  </si>
+  <si>
+    <t>• Repeat steps (e.g. data shuffle and baseline imgaug basic augmentation, train test split 70/30) from Experiment 2
+• Introduce random vertical flips for i,ii, iii, ix, x</t>
+  </si>
+  <si>
+    <t>• Perform extensive manual review of data (i.e. review past deleted images and add back if looks valid, while also reviewing existing ones to check that they are correctly labeled
+• Add sample label book data into training set
+• Adjust train/val split from 70/30 to 80/20</t>
+  </si>
+  <si>
+    <t>• Remove random order of augmentation (i.e. keep augmentation steps sequential in pre-specified order)</t>
+  </si>
+  <si>
+    <t>• Reinstate random order of augmentation
+• Adjust train/val split from 80/20 to 90/10</t>
+  </si>
+  <si>
+    <t>• Re-use steps from Experiment 4
+• Include CV2 morphological operations e.g. random erosion and dilation</t>
+  </si>
+  <si>
+    <t>• No pre-processing (Baseline)</t>
   </si>
 </sst>
 </file>
@@ -109,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="\+0.000;\-0.000;0.000"/>
+    <numFmt numFmtId="164" formatCode="\+0.000;\-0.000;0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -176,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,7 +208,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +216,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,22 +503,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="60.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6328125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -515,13 +530,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -529,16 +547,19 @@
         <v>44407</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4">
+        <v>22</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4">
         <v>0.64420999999999995</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -546,17 +567,20 @@
         <v>44407</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
         <v>0.78925999999999996</v>
       </c>
-      <c r="E3" s="9">
-        <f>D3-D2</f>
+      <c r="F3" s="9">
+        <f>E3-E2</f>
         <v>0.14505000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="124" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -564,17 +588,20 @@
         <v>44409</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4">
         <v>0.81569999999999998</v>
       </c>
-      <c r="E4" s="9">
-        <f>D4-D3</f>
+      <c r="F4" s="9">
+        <f>E4-E3</f>
         <v>2.6440000000000019E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -582,17 +609,20 @@
         <v>44409</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4">
         <v>0.82106999999999997</v>
       </c>
-      <c r="E5" s="9">
-        <f t="shared" ref="E5:E9" si="0">D5-D4</f>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F9" si="0">E5-E4</f>
         <v>5.3699999999999859E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -600,17 +630,20 @@
         <v>44414</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>0.83470999999999995</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>1.3639999999999985E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -618,17 +651,20 @@
         <v>44414</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4">
         <v>0.83967000000000003</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>4.9600000000000755E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -636,17 +672,20 @@
         <v>44414</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>0.82065999999999995</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>-1.9010000000000082E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -654,17 +693,20 @@
         <v>44415</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4">
+        <v>21</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4">
         <v>0.82438</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>3.7200000000000566E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -672,16 +714,19 @@
         <v>44415</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -689,17 +734,20 @@
         <v>44421</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
         <v>0.82809999999999995</v>
       </c>
-      <c r="E11" s="9">
-        <f>D11-D9</f>
+      <c r="F11" s="9">
+        <f>E11-E9</f>
         <v>3.7199999999999456E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="93" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -707,78 +755,91 @@
         <v>44422</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4">
+        <v>9</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4">
         <v>0.82562000000000002</v>
       </c>
-      <c r="E12" s="9">
-        <f>D12-D11</f>
+      <c r="F12" s="9">
+        <f>E12-E11</f>
         <v>-2.4799999999999267E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E9 E11:E12">
+  <conditionalFormatting sqref="F3:F9 F11:F12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>